<commit_message>
Added folders and initial files
</commit_message>
<xml_diff>
--- a/doc/Spis_czesci.xlsx
+++ b/doc/Spis_czesci.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Konsola rakieta\CRex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Konsola rakieta\CRex\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>https://www.digikey.pl/pl/products/detail/intel/10M02SCE144C8G/5284822</t>
   </si>
@@ -39,16 +39,28 @@
   </si>
   <si>
     <t>Cena za sztukę</t>
+  </si>
+  <si>
+    <t>Altera MAX 10 10M02SCE144C8G</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -72,13 +84,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -360,13 +375,13 @@
   <dimension ref="B2:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="64.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" customWidth="1"/>
+    <col min="3" max="3" width="29.77734375" customWidth="1"/>
     <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -385,11 +400,21 @@
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added some doc files
</commit_message>
<xml_diff>
--- a/doc/Spis_czesci.xlsx
+++ b/doc/Spis_czesci.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>https://www.digikey.pl/pl/products/detail/intel/10M02SCE144C8G/5284822</t>
   </si>
@@ -42,6 +42,12 @@
   </si>
   <si>
     <t>Altera MAX 10 10M02SCE144C8G</t>
+  </si>
+  <si>
+    <t>https://superelektronika.pl/pl/pamieci/247629409-k4d263238f-128m-ddr-sdram-pamiec-synchroniczna-1m-x-32bit-x-4-5905427014409.html</t>
+  </si>
+  <si>
+    <t>K4D263238F</t>
   </si>
 </sst>
 </file>
@@ -88,9 +94,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
@@ -372,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E3"/>
+  <dimension ref="B2:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -410,6 +419,17 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>

</xml_diff>

<commit_message>
Initial files for PCB
</commit_message>
<xml_diff>
--- a/doc/Spis_czesci.xlsx
+++ b/doc/Spis_czesci.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>https://www.digikey.pl/pl/products/detail/intel/10M02SCE144C8G/5284822</t>
   </si>
@@ -48,6 +48,18 @@
   </si>
   <si>
     <t>K4D263238F</t>
+  </si>
+  <si>
+    <t>https://konsolowo.pl/pl/czesci-naprawcze-joy-con/2133-analog-3d-galka-joystick-v2-joy-con-nintendo-switch-5903981901548.html</t>
+  </si>
+  <si>
+    <t>Gałka (muszkatołowa)</t>
+  </si>
+  <si>
+    <t>Triggery</t>
+  </si>
+  <si>
+    <t>https://konsolowo.pl/pl/dualsense-bdm-010/2810-triggery-adaptacyjne-haptyczne-l1-l2-r1-r2-dualsense-ps5-bdm-010-5903981916375.html</t>
   </si>
 </sst>
 </file>
@@ -94,10 +106,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -381,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E4"/>
+  <dimension ref="B2:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -430,11 +445,34 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>